<commit_message>
Exam rounds functionality added.
An exam round is a group of exams that must take place on the same day, becuase they are in fact the same exam, which is being hold multiple time for the professors due to a the lack of resources to do it all at once.
</commit_message>
<xml_diff>
--- a/files/pruebas/v6_sinFechas_3.xlsx
+++ b/files/pruebas/v6_sinFechas_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\TfgProject\files\pruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4367B530-62D4-4611-8B9B-8F17347C3CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526B3B78-9AAF-46DB-B555-6D1286020630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="420" windowWidth="26430" windowHeight="15180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="26430" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="planificación" sheetId="2" r:id="rId1"/>
@@ -2491,8 +2491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y67"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:Q29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2604,7 +2604,9 @@
       <c r="A6" s="75">
         <v>3</v>
       </c>
-      <c r="B6" s="76"/>
+      <c r="B6" s="76">
+        <v>1</v>
+      </c>
       <c r="C6" s="76" t="s">
         <v>302</v>
       </c>
@@ -6849,8 +6851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AC83AD5-6F52-41B7-9F54-B20EA3E13FEF}">
   <dimension ref="B2:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B36" sqref="B36:D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>